<commit_message>
testirana funkcija komentarisi događaj
</commit_message>
<xml_diff>
--- a/Evenizer-TestCase.xlsx
+++ b/Evenizer-TestCase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Broj testa</t>
   </si>
@@ -181,6 +181,9 @@
     <t>7.1.2020.</t>
   </si>
   <si>
+    <t>Isprobano je i dodavanje već postojećeg događaja.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -201,22 +204,58 @@
         <charset val="238"/>
       </rPr>
       <t xml:space="preserve">
-Test za utvrđivanje da li se korisnik može dodati novi događaj. Pri pokušaju dodavanja događaja korisnik unosi podatke o događaju. Svi podaci osim specijalnih zahtjeva su obavezni.</t>
+Test za utvrđivanje da li korisnik može dodati novi događaj. Pri pokušaju dodavanja događaja korisnik unosi podatke o događaju. Svi podaci osim specijalnih zahtjeva su obavezni.</t>
     </r>
   </si>
   <si>
-    <t>Isprobano je i dodavanje već postojećeg događaja.</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Komentarisanje događaja</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">
+Test za utvrđivanje da li  korisnik može komentarisati neki događaj. Pri pokušaju komentarisanja događaja korisnik unosi naziv događaja i komentar.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. unos naziva događaja i komentara
+3. odabir opcije "Komentariši"</t>
+  </si>
+  <si>
+    <t>Isprobano je i komentarisanje nepostojećeg događaja.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
@@ -291,9 +330,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,41 +341,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -648,7 +693,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
@@ -853,12 +898,40 @@
         <v>13</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="J7" s="15"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>

</xml_diff>

<commit_message>
testirane funkcije removeComment banUser getCategories changeCategories
</commit_message>
<xml_diff>
--- a/Evenizer-TestCase.xlsx
+++ b/Evenizer-TestCase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Broj testa</t>
   </si>
@@ -143,10 +143,6 @@
     <t>1. instalirana aplikacija 2. korisnik mora biti ulogovan</t>
   </si>
   <si>
-    <t>1. unos željenih parametara za filtriranje i prikaz događaja
-3. odabir opcije "Pretraži"</t>
-  </si>
-  <si>
     <t>Provjerene sve moguće kombinacije parametara pretrage događaja.</t>
   </si>
   <si>
@@ -174,10 +170,6 @@
     </r>
   </si>
   <si>
-    <t>1. unos podataka o novom događaju
-3. odabir opcije "Dodaj"</t>
-  </si>
-  <si>
     <t>7.1.2020.</t>
   </si>
   <si>
@@ -232,22 +224,142 @@
     </r>
   </si>
   <si>
+    <t>Isprobano je i komentarisanje nepostojećeg događaja.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Banovanje korisnika</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">
+Test za utvrđivanje da li  administrator može banovati nekog registrovanog korisnika. Pri pokušaju banovanja administrator unosi korisničko ime korisnika kojeg želi banovati.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. instalirana aplikacija 2. korisnik mora biti ulogovani administrator</t>
+  </si>
+  <si>
+    <t>Za već banovanog korisnika ispis je da korisnik sa datim imenom ne postoji.</t>
+  </si>
+  <si>
+    <t>Provjeriti da li je korisnik već banovan.</t>
+  </si>
+  <si>
+    <t>1. unos željenih parametara za filtriranje i prikaz događaja
+2. odabir opcije "Pretraži"</t>
+  </si>
+  <si>
+    <t>1. unos podataka o novom događaju
+2. odabir opcije "Dodaj"</t>
+  </si>
+  <si>
     <t>1. unos naziva događaja i komentara
-3. odabir opcije "Komentariši"</t>
-  </si>
-  <si>
-    <t>Isprobano je i komentarisanje nepostojećeg događaja.</t>
+2. odabir opcije "Komentariši"</t>
+  </si>
+  <si>
+    <t>1. unos korisničkog imena korisnika koji treba biti banovan
+2. odabir opcije "Banuj"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Pribavljanje i izmjena kategorija</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">
+Test za utvrđivanje da li  korisnik može mijenjati postojeće kategorije. Pri pokušaju izmjene kategorija korisnik unosi spisak kategorija ukljucujuci i stare.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. unos kompletne liste kategorija
+2. odabir opcije "Izmjeni"</t>
+  </si>
+  <si>
+    <t>Isprobano je i unošenje već postojećih kategorija.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>Uklanjanje komentara</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">
+Test za utvrđivanje da li  administrator može ukloniti komentar na nekom događaju. Pri pokušaju uklanjanja komentara administrator unosi naziv događaja i komentar koji želi ukloniti.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. unos komentara i naziva događaja
+2. odabir opcije "Ukloni"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
@@ -330,9 +442,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -341,41 +453,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -692,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,13 +960,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
+      <c r="D5" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
@@ -866,7 +984,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -874,13 +992,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>31</v>
+      <c r="D6" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>11</v>
@@ -888,8 +1006,8 @@
       <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>32</v>
+      <c r="G6" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>19</v>
@@ -897,8 +1015,8 @@
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>33</v>
+      <c r="J6" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -906,13 +1024,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
@@ -920,8 +1038,8 @@
       <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>32</v>
+      <c r="G7" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>19</v>
@@ -929,37 +1047,147 @@
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="J8" s="15"/>
+      <c r="G8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="J11" s="15"/>
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>